<commit_message>
spr 20240604 transient local change added
</commit_message>
<xml_diff>
--- a/MMN/MSTI_ClickTrain_Config.xlsx
+++ b/MMN/MSTI_ClickTrain_Config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8AEF48-3F92-4288-88DE-B06A5E2C668C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D825A3-F690-4F43-A592-D91E2A467D1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="194">
   <si>
     <t>Amp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -528,6 +528,259 @@
   </si>
   <si>
     <t>Ascend_4ms_Dur300ms.wav,Descend_4ms_Dur300ms.wav,Jitter0-20_ICI_4ms.wav,Jitter10-10_ICI_4ms.wav,Jitter30-30_ICI_4ms.wav,Jitter20-40_ICI_4ms.wav,Jitter50-50_ICI_4ms.wav,Jitter40-60_ICI_4ms.wav,Jitter70-70_ICI_4ms.wav,Regular_4ms_Dur300ms.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024/03/1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_STD-4_4o06_DEV-4o06_4_STDN_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HumanEEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Reg_Dur600_4-4o06_No-Rep.wav,TB_Reg_Dur601.25_4o06-4_No-Rep.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>successive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\HumanEEG\2024-03-01_HumanEEG_Oddball_Pool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_Block_STD-4_4o06_DEV-4o06_4_STDN_9</t>
+  </si>
+  <si>
+    <t>Oddball_Block_STD-4_4o06_DEV-4o06_4_STDN_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024/05/28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Amp_STDN_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\HumanEEG\2024-05-28_ComplexTone Frequency Local Change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0_Freqs-1000-2000-4000-8000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.01_Freqs-1000-2000-4000-8000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.02_Freqs-1000-2000-4000-8000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.04_Freqs-1000-2000-4000-8000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.08_Freqs-1000-2000-4000-8000.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Amp_STDN_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Amp_STDN_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\HumanEEG\2024-05-28_ComplexTone Amplitude Local Change</t>
+  </si>
+  <si>
+    <t>E:\sounds\HumanEEG\2024-05-28_ComplexTone Amplitude Local Change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.1_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.2_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.4_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.8_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav</t>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.1_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.2_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.4_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Amp-0.8_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024/05/29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\HumanEEG\2024-05-29_ComplexTone Frequency Local Change</t>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.01_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.02_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.03_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0.04_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ManyStd_RandIdx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq-0_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq--0.01_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq--0.02_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq--0.03_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-150ms_Dur-2ms_Freq--0.04_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-300ms_LocalChange-0ms_Dur-300ms_Freq--0.05_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-0ms_Dur-300ms_Freq--0.1_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-0ms_Dur-300ms_Freq--0.15_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-0ms_Dur-300ms_Freq--0.2_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav,ComplexTone_Dur-300ms_LocalChange-0ms_Dur-300ms_Freq--0.25_Freqs-500-731-1070-1565-2289-3349-4899-7166-10483-15335-22432-32813-48000.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\HumanEEG\2024-05-30_ComplexTone Frequency Local Change</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024/05/31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\monkeySounds\2024-05-31_ComplexTone Frequency Local Change</t>
+  </si>
+  <si>
+    <t>monkeySounds</t>
+  </si>
+  <si>
+    <t>monkeySounds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>700</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-400ms_LocalChange-0ms_Dur-400ms_Freq--0.05_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-0ms_Dur-400ms_Freq--0.1_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-0ms_Dur-400ms_Freq--0.15_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-0ms_Dur-400ms_Freq--0.2_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-0ms_Dur-400ms_Freq--0.25_Freqs-500-48000-N13.wav</t>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last6_400ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last3_400ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last1_400ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last1_300ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last3_300ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_6_Last9_400ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq-0_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.009_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.018_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.027_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.036_Freqs-500-48000-N13.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq-0_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.01_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.02_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.03_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.04_Freqs-500-48000-N13.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\monkeySounds\2024-06-02_ComplexTone Frequency Local Change_400ms</t>
+  </si>
+  <si>
+    <t>2024/06/03</t>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_9_Last9_400ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_9_Last3_400ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_9_Last1_400ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_9_Last9_400ms_V4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_9_Last3_400ms_V4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oddball_LocalChange_Freq_STDN_9_Last1_400ms_V4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\sounds\monkeySounds\2024-06-03_ComplexTone Frequency Local Change_400ms</t>
+  </si>
+  <si>
+    <t>ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq-0_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.018_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.022_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.026_Freqs-500-48000-N13.wav,ComplexTone_Dur-400ms_LocalChange-200ms_Dur-2ms_Freq--0.03_Freqs-500-48000-N13.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,7 +822,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,8 +841,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -692,60 +951,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -755,11 +1081,171 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1040,1663 +1526,3388 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y31" sqref="Y31"/>
+    <sheetView tabSelected="1" topLeftCell="U55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z57" sqref="Z57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45" style="2" customWidth="1"/>
-    <col min="6" max="6" width="61.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.77734375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="14" style="3" customWidth="1"/>
-    <col min="19" max="19" width="26.33203125" style="3" customWidth="1"/>
-    <col min="20" max="20" width="68.88671875" style="7" customWidth="1"/>
-    <col min="21" max="21" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" customWidth="1"/>
-    <col min="23" max="23" width="24" style="20" customWidth="1"/>
-    <col min="24" max="25" width="17.33203125" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="8.375" style="37" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" style="37" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="8"/>
+    <col min="6" max="6" width="61.375" style="37" customWidth="1"/>
+    <col min="7" max="7" width="19.875" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.375" style="38" customWidth="1"/>
+    <col min="9" max="9" width="8.125" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.875" style="1" customWidth="1"/>
+    <col min="11" max="13" width="17.5" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16.875" style="38" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.75" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="1" customWidth="1"/>
+    <col min="21" max="21" width="26.375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="102.125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="24" style="7" customWidth="1"/>
+    <col min="26" max="26" width="72.125" style="8" customWidth="1"/>
+    <col min="27" max="27" width="68" style="8" customWidth="1"/>
+    <col min="28" max="28" width="18.375" style="9" customWidth="1"/>
+    <col min="29" max="16384" width="8.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="11" t="s">
+      <c r="I1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="O1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="P1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="Q1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="S1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="T1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="U1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="V1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="W1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="X1" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="Y1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="X1" s="41" t="s">
+      <c r="Z1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="42" t="s">
+      <c r="AA1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="AB1" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
-        <v>0</v>
-      </c>
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="1:28" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="N2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="O2" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="Q2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="R2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="30" t="s">
+      <c r="S2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="30" t="s">
+      <c r="T2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="U2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="V2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="32" t="s">
+      <c r="W2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="32" t="s">
+      <c r="X2" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="W2" s="43" t="s">
+      <c r="Y2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="X2" s="26" t="s">
+      <c r="Z2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="AA2" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="Z2" s="35" t="s">
+      <c r="AB2" s="35" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="37">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>97656</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="37">
         <v>0.5</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="8">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="P3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="R3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="S3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="3">
-        <v>1</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="V3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="36" t="s">
+      <c r="AB3" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="37">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>97656</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="37">
         <v>0.5</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="8">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="S4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="3">
-        <v>1</v>
-      </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="V4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="36" t="s">
+      <c r="AB4" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="37">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>97656</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="37">
         <v>0.5</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="8">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="O5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="P5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="Q5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="R5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="S5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="3">
-        <v>1</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="V5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z5" s="36" t="s">
+      <c r="AB5" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="37">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>97656</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="37">
         <v>0.5</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="8">
-        <v>1</v>
-      </c>
-      <c r="L6" s="5" t="s">
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="O6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="P6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="Q6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="R6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="S6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="3">
-        <v>1</v>
-      </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="V6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z6" s="36" t="s">
+      <c r="AB6" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="37">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>97656</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="37">
         <v>0.5</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="8">
-        <v>1</v>
-      </c>
-      <c r="L7" s="5" t="s">
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="O7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="P7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="Q7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="R7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="S7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="R7" s="3">
-        <v>1</v>
-      </c>
-      <c r="S7" s="3" t="s">
+      <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T7" s="7" t="s">
+      <c r="V7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U7" t="s">
+      <c r="W7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z7" s="36" t="s">
+      <c r="AB7" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="37">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>97656</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="37">
         <v>0.5</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="8">
-        <v>1</v>
-      </c>
-      <c r="L8" s="5" t="s">
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="O8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="P8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="Q8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="R8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="S8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="R8" s="3">
-        <v>1</v>
-      </c>
-      <c r="S8" s="3" t="s">
+      <c r="T8" s="1">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T8" s="7" t="s">
+      <c r="V8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z8" s="36" t="s">
+      <c r="AB8" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" s="37">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>97656</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="37">
         <v>0.5</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K9" s="8">
-        <v>1</v>
-      </c>
-      <c r="L9" s="5" t="s">
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="P9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="Q9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="R9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="S9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R9" s="3">
-        <v>1</v>
-      </c>
-      <c r="S9" s="3" t="s">
+      <c r="T9" s="1">
+        <v>1</v>
+      </c>
+      <c r="U9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="T9" s="7" t="s">
+      <c r="V9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z9" s="36" t="s">
+      <c r="AB9" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" s="37">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>97656</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="37">
         <v>0.5</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K10" s="8">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5" t="s">
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="O10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="P10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="Q10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="R10" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="S10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="R10" s="3">
-        <v>1</v>
-      </c>
-      <c r="S10" s="3" t="s">
+      <c r="T10" s="1">
+        <v>1</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="T10" s="7" t="s">
+      <c r="V10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U10" t="s">
+      <c r="W10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z10" s="36" t="s">
+      <c r="AB10" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" s="37">
         <v>9.1</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>97656</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="37">
         <v>0.5</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="8">
-        <v>1</v>
-      </c>
-      <c r="L11" s="5" t="s">
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="O11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="P11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="Q11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="R11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="S11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R11" s="3">
-        <v>1</v>
-      </c>
-      <c r="S11" s="3" t="s">
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="V11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z11" s="36" t="s">
+      <c r="AB11" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="37">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>97656</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="37">
         <v>0.5</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="8">
-        <v>1</v>
-      </c>
-      <c r="L12" s="5" t="s">
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="O12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="P12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="Q12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="R12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="S12" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R12" s="3">
-        <v>1</v>
-      </c>
-      <c r="S12" s="3" t="s">
+      <c r="T12" s="1">
+        <v>1</v>
+      </c>
+      <c r="U12" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="T12" s="7" t="s">
+      <c r="V12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U12" t="s">
+      <c r="W12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z12" s="36" t="s">
+      <c r="AB12" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="37">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
         <v>97656</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="37">
         <v>0.5</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K13" s="8">
-        <v>1</v>
-      </c>
-      <c r="L13" s="5" t="s">
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="O13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="P13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="Q13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="R13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="S13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R13" s="3">
-        <v>1</v>
-      </c>
-      <c r="S13" s="3" t="s">
+      <c r="T13" s="1">
+        <v>1</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="T13" s="7" t="s">
+      <c r="V13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U13" t="s">
+      <c r="W13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z13" s="36" t="s">
+      <c r="AB13" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="37">
         <v>9.4</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>97656</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="37">
         <v>0.5</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K14" s="8">
-        <v>1</v>
-      </c>
-      <c r="L14" s="5" t="s">
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="O14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="P14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="Q14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="R14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="S14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R14" s="3">
-        <v>1</v>
-      </c>
-      <c r="S14" s="3" t="s">
+      <c r="T14" s="1">
+        <v>1</v>
+      </c>
+      <c r="U14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="T14" s="7" t="s">
+      <c r="V14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U14" t="s">
+      <c r="W14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z14" s="36" t="s">
+      <c r="AB14" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" s="37">
         <v>9.5</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>97656</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="37">
         <v>0.5</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K15" s="8">
-        <v>1</v>
-      </c>
-      <c r="L15" s="5" t="s">
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="O15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="P15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="Q15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="R15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Q15" s="3" t="s">
+      <c r="S15" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R15" s="3">
-        <v>1</v>
-      </c>
-      <c r="S15" s="3" t="s">
+      <c r="T15" s="1">
+        <v>1</v>
+      </c>
+      <c r="U15" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="T15" s="7" t="s">
+      <c r="V15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U15" t="s">
+      <c r="W15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z15" s="36" t="s">
+      <c r="AB15" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" s="37">
         <v>9.6</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="2">
         <v>97656</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="37">
         <v>0.5</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="8">
-        <v>1</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="O16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="P16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="Q16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="R16" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="S16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R16" s="3">
-        <v>1</v>
-      </c>
-      <c r="S16" s="3" t="s">
+      <c r="T16" s="1">
+        <v>1</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="T16" s="7" t="s">
+      <c r="V16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U16" t="s">
+      <c r="W16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Z16" s="36" t="s">
+      <c r="AB16" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="138" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="17" spans="1:28" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="39">
         <v>101</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="40">
         <v>97656</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="39">
         <v>0.5</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K17" s="8">
-        <v>1</v>
-      </c>
-      <c r="W17" s="37" t="s">
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="X17" s="38" t="s">
+      <c r="Z17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="Y17" s="38" t="s">
+      <c r="AA17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="Z17" s="39" t="s">
+      <c r="AB17" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="18" spans="1:28" ht="57" x14ac:dyDescent="0.2">
+      <c r="A18" s="39">
         <v>101.1</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="40">
         <v>97656</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="39">
         <v>0.5</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="8">
-        <v>0</v>
-      </c>
-      <c r="W18" s="37" t="s">
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="X18" s="38" t="s">
+      <c r="Z18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Y18" s="38" t="s">
+      <c r="AA18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Z18" s="39" t="s">
+      <c r="AB18" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+    <row r="19" spans="1:28" ht="57" x14ac:dyDescent="0.2">
+      <c r="A19" s="39">
         <v>101.2</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="40">
         <v>97656</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="39">
         <v>0.5</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="8">
-        <v>0</v>
-      </c>
-      <c r="W19" s="37" t="s">
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="X19" s="38" t="s">
+      <c r="Z19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Y19" s="38" t="s">
+      <c r="AA19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Z19" s="39" t="s">
+      <c r="AB19" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+    <row r="20" spans="1:28" ht="57" x14ac:dyDescent="0.2">
+      <c r="A20" s="39">
         <v>101.3</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="40">
         <v>97656</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="39">
         <v>0.5</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K20" s="8">
-        <v>0</v>
-      </c>
-      <c r="W20" s="37" t="s">
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="X20" s="38" t="s">
+      <c r="Z20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Y20" s="38" t="s">
+      <c r="AA20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Z20" s="39" t="s">
+      <c r="AB20" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+    <row r="21" spans="1:28" ht="57" x14ac:dyDescent="0.2">
+      <c r="A21" s="39">
         <v>101.4</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="40">
         <v>97656</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="39">
         <v>0.5</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K21" s="8">
-        <v>0</v>
-      </c>
-      <c r="W21" s="37" t="s">
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="X21" s="38" t="s">
+      <c r="Z21" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Y21" s="38" t="s">
+      <c r="AA21" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Z21" s="39" t="s">
+      <c r="AB21" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+    <row r="22" spans="1:28" ht="57" x14ac:dyDescent="0.2">
+      <c r="A22" s="39">
         <v>101.5</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="40">
         <v>97656</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="39">
         <v>0.5</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K22" s="8">
-        <v>0</v>
-      </c>
-      <c r="W22" s="37" t="s">
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="X22" s="38" t="s">
+      <c r="Z22" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Y22" s="38" t="s">
+      <c r="AA22" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Z22" s="39" t="s">
+      <c r="AB22" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="207.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+    <row r="23" spans="1:28" ht="207.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="39">
         <v>102</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="40">
         <v>97656</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="39">
         <v>0.5</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K23" s="8">
-        <v>0</v>
-      </c>
-      <c r="V23">
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="X23" s="8">
         <v>30</v>
       </c>
-      <c r="W23" s="37" t="s">
+      <c r="Y23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="X23" s="38" t="s">
+      <c r="Z23" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Y23" s="38" t="s">
+      <c r="AA23" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="Z23" s="39" t="s">
+      <c r="AB23" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+    <row r="24" spans="1:28" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="39">
         <v>102.1</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="40">
         <v>97656</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="39">
         <v>0.5</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K24" s="8">
-        <v>0</v>
-      </c>
-      <c r="V24">
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0</v>
+      </c>
+      <c r="X24" s="8">
         <v>30</v>
       </c>
-      <c r="W24" s="37" t="s">
+      <c r="Y24" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="X24" s="38" t="s">
+      <c r="Z24" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="Y24" s="38" t="s">
+      <c r="AA24" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="Z24" s="39" t="s">
+      <c r="AB24" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="207.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+    <row r="25" spans="1:28" ht="207.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="39">
         <v>102.2</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="40">
         <v>97656</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="E25" s="8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="39">
         <v>0.5</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K25" s="8">
-        <v>0</v>
-      </c>
-      <c r="V25">
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0</v>
+      </c>
+      <c r="X25" s="8">
         <v>30</v>
       </c>
-      <c r="W25" s="37" t="s">
+      <c r="Y25" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X25" s="38" t="s">
+      <c r="Z25" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Y25" s="38" t="s">
+      <c r="AA25" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="Z25" s="39" t="s">
+      <c r="AB25" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+    <row r="26" spans="1:28" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="39">
         <v>102.3</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="40">
         <v>97656</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="39">
         <v>0.5</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="8">
-        <v>0</v>
-      </c>
-      <c r="V26">
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="X26" s="8">
         <v>30</v>
       </c>
-      <c r="W26" s="37" t="s">
+      <c r="Y26" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X26" s="38" t="s">
+      <c r="Z26" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="Y26" s="38" t="s">
+      <c r="AA26" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="Z26" s="39" t="s">
+      <c r="AB26" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="I33" s="6"/>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="I34" s="6"/>
+    <row r="27" spans="1:28" ht="57" x14ac:dyDescent="0.2">
+      <c r="A27" s="39">
+        <v>201</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="I27" s="39">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z27" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="39">
+        <v>202</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" s="39">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z28" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB28" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="Y29" s="44"/>
+      <c r="AB29" s="45"/>
+    </row>
+    <row r="30" spans="1:28" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="41"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="Y30" s="44"/>
+      <c r="AB30" s="45"/>
+    </row>
+    <row r="31" spans="1:28" ht="171" x14ac:dyDescent="0.2">
+      <c r="A31" s="39">
+        <v>301</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="8">
+        <v>1</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="I31" s="39">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z31" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA31" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB31" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" ht="171" x14ac:dyDescent="0.2">
+      <c r="A32" s="39">
+        <v>301.10000000000002</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" s="39">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z32" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA32" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB32" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" ht="171" x14ac:dyDescent="0.2">
+      <c r="A33" s="39">
+        <v>301.2</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H33" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I33" s="39">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z33" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA33" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB33" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="39">
+        <v>302</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="39">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z34" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB34" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="39">
+        <v>302.10000000000002</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="8">
+        <v>1</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H35" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" s="39">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z35" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB35" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="39">
+        <v>302.2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="8">
+        <v>1</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="G36" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36" s="39">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z36" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB36" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="39">
+        <v>303</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="8">
+        <v>1</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I37" s="39">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z37" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB37" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="39">
+        <v>303.10000000000002</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H38" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I38" s="39">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K38" s="2">
+        <v>0</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z38" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB38" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="39">
+        <v>303.2</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="8">
+        <v>1</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="39">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z39" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB39" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="39">
+        <v>304</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H40" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="I40" s="39">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z40" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA40" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB40" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="39">
+        <v>304.10000000000002</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" s="8">
+        <v>1</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" s="39">
+        <v>1</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M41" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z41" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA41" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB41" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="39">
+        <v>304.2</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="40">
+        <v>384000</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" s="8">
+        <v>1</v>
+      </c>
+      <c r="F42" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H42" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I42" s="39">
+        <v>1</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K42" s="2">
+        <v>1</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M42" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z42" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA42" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB42" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="39">
+        <v>304.3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="8">
+        <v>1</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="G43" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H43" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="I43" s="39">
+        <v>1</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K43" s="2">
+        <v>0</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0</v>
+      </c>
+      <c r="M43" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z43" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA43" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB43" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="39">
+        <v>304.39999999999998</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" s="8">
+        <v>1</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H44" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I44" s="39">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M44" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z44" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA44" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB44" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="39">
+        <v>304.5</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="E45" s="8">
+        <v>1</v>
+      </c>
+      <c r="F45" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="G45" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H45" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" s="39">
+        <v>1</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M45" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z45" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA45" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB45" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="39">
+        <v>304.60000000000002</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="8">
+        <v>1</v>
+      </c>
+      <c r="F46" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G46" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H46" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I46" s="39">
+        <v>1</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0</v>
+      </c>
+      <c r="L46" s="2">
+        <v>0</v>
+      </c>
+      <c r="M46" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z46" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA46" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB46" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="39">
+        <v>304.7</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D47" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" s="8">
+        <v>1</v>
+      </c>
+      <c r="F47" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H47" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I47" s="39">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K47" s="2">
+        <v>1</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M47" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z47" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA47" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB47" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="39">
+        <v>304.8</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D48" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="E48" s="8">
+        <v>1</v>
+      </c>
+      <c r="F48" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="G48" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H48" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I48" s="39">
+        <v>1</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M48" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z48" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA48" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB48" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="39">
+        <v>304.89999999999998</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D49" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="E49" s="8">
+        <v>1</v>
+      </c>
+      <c r="F49" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H49" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I49" s="39">
+        <v>1</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0</v>
+      </c>
+      <c r="L49" s="2">
+        <v>0</v>
+      </c>
+      <c r="M49" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z49" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA49" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB49" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="39">
+        <v>304.11</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="8">
+        <v>1</v>
+      </c>
+      <c r="F50" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="G50" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H50" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I50" s="39">
+        <v>1</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K50" s="2">
+        <v>1</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M50" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z50" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA50" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB50" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" ht="100.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="39">
+        <v>304.12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D51" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E51" s="8">
+        <v>1</v>
+      </c>
+      <c r="F51" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="G51" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H51" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I51" s="39">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M51" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z51" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA51" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB51" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" s="50" customFormat="1" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="46">
+        <v>304.13</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="48">
+        <v>97656</v>
+      </c>
+      <c r="D52" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="E52" s="50">
+        <v>1</v>
+      </c>
+      <c r="F52" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="G52" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="H52" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="I52" s="49">
+        <v>1</v>
+      </c>
+      <c r="J52" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="K52" s="52">
+        <v>0</v>
+      </c>
+      <c r="L52" s="52">
+        <v>0</v>
+      </c>
+      <c r="M52" s="52">
+        <v>0</v>
+      </c>
+      <c r="N52" s="51"/>
+      <c r="O52" s="47"/>
+      <c r="P52" s="47"/>
+      <c r="Q52" s="47"/>
+      <c r="R52" s="47"/>
+      <c r="S52" s="47"/>
+      <c r="T52" s="47"/>
+      <c r="U52" s="47"/>
+      <c r="V52" s="47"/>
+      <c r="Y52" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z52" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA52" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB52" s="54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" s="37" customFormat="1" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="55">
+        <v>304.14</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="E53" s="37">
+        <v>1</v>
+      </c>
+      <c r="F53" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="G53" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H53" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I53" s="39">
+        <v>1</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K53" s="2">
+        <v>1</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M53" s="2">
+        <v>0</v>
+      </c>
+      <c r="N53" s="38"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="Y53" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z53" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA53" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB53" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" s="60" customFormat="1" ht="100.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="56">
+        <v>304.14999999999998</v>
+      </c>
+      <c r="B54" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="58">
+        <v>97656</v>
+      </c>
+      <c r="D54" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="E54" s="60">
+        <v>1</v>
+      </c>
+      <c r="F54" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="G54" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="H54" s="61" t="s">
+        <v>172</v>
+      </c>
+      <c r="I54" s="59">
+        <v>1</v>
+      </c>
+      <c r="J54" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="K54" s="62">
+        <v>1</v>
+      </c>
+      <c r="L54" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="M54" s="62">
+        <v>0</v>
+      </c>
+      <c r="N54" s="61"/>
+      <c r="O54" s="57"/>
+      <c r="P54" s="57"/>
+      <c r="Q54" s="57"/>
+      <c r="R54" s="57"/>
+      <c r="S54" s="57"/>
+      <c r="T54" s="57"/>
+      <c r="U54" s="57"/>
+      <c r="V54" s="57"/>
+      <c r="Y54" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z54" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA54" s="60" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB54" s="64" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="39">
+        <v>304.16000000000003</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D55" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="E55" s="8">
+        <v>1</v>
+      </c>
+      <c r="F55" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H55" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I55" s="39">
+        <v>1</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K55" s="2">
+        <v>0</v>
+      </c>
+      <c r="L55" s="2">
+        <v>0</v>
+      </c>
+      <c r="M55" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y55" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z55" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA55" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB55" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="39">
+        <v>304.17</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D56" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="E56" s="8">
+        <v>1</v>
+      </c>
+      <c r="F56" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="G56" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H56" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I56" s="39">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K56" s="2">
+        <v>1</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M56" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z56" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA56" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB56" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="39">
+        <v>304.18</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" s="40">
+        <v>97656</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="E57" s="8">
+        <v>1</v>
+      </c>
+      <c r="F57" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="G57" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H57" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I57" s="39">
+        <v>1</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K57" s="2">
+        <v>1</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M57" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z57" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA57" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB57" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>